<commit_message>
va_emerging_tech - revised scenarios and analysis
combined_analysis.py  - fixed problem with LCOE and avgEmissions, previously no output was provided
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/analyze_inputs/ATB_data_analysis/2020_ATB_CostProjections.xlsx
+++ b/projects/va_emerging_tech/analyze_inputs/ATB_data_analysis/2020_ATB_CostProjections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\coopercenter_temoatools\projects\va_emerging_tech\analyze_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\coopercenter_temoatools\projects\va_emerging_tech\analyze_inputs\ATB_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630E9C34-E7E1-4C13-9B99-431E8B64714C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969984B3-5B81-470B-B270-409190E2A96E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="889" firstSheet="5" activeTab="14" xr2:uid="{EBBDE126-F62A-45CA-A9F5-DC77CD44D7C9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="889" firstSheet="4" activeTab="15" xr2:uid="{EBBDE126-F62A-45CA-A9F5-DC77CD44D7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Coal_new" sheetId="24" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Battery_2hr" sheetId="21" r:id="rId13"/>
     <sheet name="Nuclear" sheetId="26" r:id="rId14"/>
     <sheet name="Hydro_NPD4" sheetId="27" r:id="rId15"/>
+    <sheet name="Coal_IGCC" sheetId="28" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -7672,8 +7673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97998281-4CAD-4EFF-95EE-DE2F5ADDD260}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8720,6 +8721,1061 @@
       </c>
       <c r="AH10" s="79">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EAE330-8560-4191-9086-78932A7833DD}">
+  <dimension ref="A1:AH10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AH10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:34">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="4">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G1" s="4">
+        <v>2023</v>
+      </c>
+      <c r="H1" s="4">
+        <v>2024</v>
+      </c>
+      <c r="I1" s="4">
+        <v>2025</v>
+      </c>
+      <c r="J1" s="4">
+        <v>2026</v>
+      </c>
+      <c r="K1" s="4">
+        <v>2027</v>
+      </c>
+      <c r="L1" s="4">
+        <v>2028</v>
+      </c>
+      <c r="M1" s="4">
+        <v>2029</v>
+      </c>
+      <c r="N1" s="4">
+        <v>2030</v>
+      </c>
+      <c r="O1" s="4">
+        <v>2031</v>
+      </c>
+      <c r="P1" s="4">
+        <v>2032</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>2033</v>
+      </c>
+      <c r="R1" s="4">
+        <v>2034</v>
+      </c>
+      <c r="S1" s="4">
+        <v>2035</v>
+      </c>
+      <c r="T1" s="4">
+        <v>2036</v>
+      </c>
+      <c r="U1" s="4">
+        <v>2037</v>
+      </c>
+      <c r="V1" s="4">
+        <v>2038</v>
+      </c>
+      <c r="W1" s="4">
+        <v>2039</v>
+      </c>
+      <c r="X1" s="4">
+        <v>2040</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>2041</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>2042</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>2043</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>2044</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>2045</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>2046</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>2047</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>2048</v>
+      </c>
+      <c r="AG1" s="4">
+        <v>2049</v>
+      </c>
+      <c r="AH1" s="4">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
+      <c r="A2" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="79">
+        <v>4740.3058669850725</v>
+      </c>
+      <c r="C2" s="79">
+        <v>4698.4718301828261</v>
+      </c>
+      <c r="D2" s="79">
+        <v>4656.6377933805788</v>
+      </c>
+      <c r="E2" s="79">
+        <v>4614.8037565783325</v>
+      </c>
+      <c r="F2" s="79">
+        <v>4572.9697197760852</v>
+      </c>
+      <c r="G2" s="79">
+        <v>4492.3388421270865</v>
+      </c>
+      <c r="H2" s="79">
+        <v>4450.5048053248402</v>
+      </c>
+      <c r="I2" s="79">
+        <v>4425.919733817439</v>
+      </c>
+      <c r="J2" s="79">
+        <v>4401.1503622317005</v>
+      </c>
+      <c r="K2" s="79">
+        <v>4375.6027304194013</v>
+      </c>
+      <c r="L2" s="79">
+        <v>4353.7695723430206</v>
+      </c>
+      <c r="M2" s="79">
+        <v>4323.0632929515905</v>
+      </c>
+      <c r="N2" s="79">
+        <v>4303.5989948717279</v>
+      </c>
+      <c r="O2" s="79">
+        <v>4285.2818354981382</v>
+      </c>
+      <c r="P2" s="79">
+        <v>4262.0324883591757</v>
+      </c>
+      <c r="Q2" s="79">
+        <v>4242.8368257164166</v>
+      </c>
+      <c r="R2" s="79">
+        <v>4225.3148592700782</v>
+      </c>
+      <c r="S2" s="79">
+        <v>4204.5718557405344</v>
+      </c>
+      <c r="T2" s="79">
+        <v>4184.3718456945344</v>
+      </c>
+      <c r="U2" s="79">
+        <v>4165.798924455009</v>
+      </c>
+      <c r="V2" s="79">
+        <v>4152.0220751579782</v>
+      </c>
+      <c r="W2" s="79">
+        <v>4136.0312119601085</v>
+      </c>
+      <c r="X2" s="79">
+        <v>4120.5639552154853</v>
+      </c>
+      <c r="Y2" s="79">
+        <v>4109.3400307856145</v>
+      </c>
+      <c r="Z2" s="79">
+        <v>4088.851743916076</v>
+      </c>
+      <c r="AA2" s="79">
+        <v>4079.7552383590519</v>
+      </c>
+      <c r="AB2" s="79">
+        <v>4060.153754291312</v>
+      </c>
+      <c r="AC2" s="79">
+        <v>4050.1467204692653</v>
+      </c>
+      <c r="AD2" s="79">
+        <v>4032.1404971157867</v>
+      </c>
+      <c r="AE2" s="79">
+        <v>4017.8938145366546</v>
+      </c>
+      <c r="AF2" s="79">
+        <v>4003.5815606324636</v>
+      </c>
+      <c r="AG2" s="79">
+        <v>3988.9113124344767</v>
+      </c>
+      <c r="AH2" s="79">
+        <v>3943.6089504257593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
+      <c r="A3" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="79">
+        <v>4740.3058669850725</v>
+      </c>
+      <c r="C3" s="79">
+        <v>4698.4718301828261</v>
+      </c>
+      <c r="D3" s="79">
+        <v>4656.6377933805788</v>
+      </c>
+      <c r="E3" s="79">
+        <v>4614.8037565783325</v>
+      </c>
+      <c r="F3" s="79">
+        <v>4572.9697197760852</v>
+      </c>
+      <c r="G3" s="79">
+        <v>4492.3388421270865</v>
+      </c>
+      <c r="H3" s="79">
+        <v>4450.5048053248402</v>
+      </c>
+      <c r="I3" s="79">
+        <v>4425.919733817439</v>
+      </c>
+      <c r="J3" s="79">
+        <v>4401.1503622317005</v>
+      </c>
+      <c r="K3" s="79">
+        <v>4375.6027304194013</v>
+      </c>
+      <c r="L3" s="79">
+        <v>4353.7695723430206</v>
+      </c>
+      <c r="M3" s="79">
+        <v>4323.0632929515905</v>
+      </c>
+      <c r="N3" s="79">
+        <v>4303.5989948717279</v>
+      </c>
+      <c r="O3" s="79">
+        <v>4285.2818354981382</v>
+      </c>
+      <c r="P3" s="79">
+        <v>4262.0324883591757</v>
+      </c>
+      <c r="Q3" s="79">
+        <v>4242.8368257164166</v>
+      </c>
+      <c r="R3" s="79">
+        <v>4225.3148592700782</v>
+      </c>
+      <c r="S3" s="79">
+        <v>4204.5718557405344</v>
+      </c>
+      <c r="T3" s="79">
+        <v>4184.3718456945344</v>
+      </c>
+      <c r="U3" s="79">
+        <v>4165.798924455009</v>
+      </c>
+      <c r="V3" s="79">
+        <v>4152.0220751579782</v>
+      </c>
+      <c r="W3" s="79">
+        <v>4136.0312119601085</v>
+      </c>
+      <c r="X3" s="79">
+        <v>4120.5639552154853</v>
+      </c>
+      <c r="Y3" s="79">
+        <v>4109.3400307856145</v>
+      </c>
+      <c r="Z3" s="79">
+        <v>4088.851743916076</v>
+      </c>
+      <c r="AA3" s="79">
+        <v>4079.7552383590519</v>
+      </c>
+      <c r="AB3" s="79">
+        <v>4060.153754291312</v>
+      </c>
+      <c r="AC3" s="79">
+        <v>4050.1467204692653</v>
+      </c>
+      <c r="AD3" s="79">
+        <v>4032.1404971157867</v>
+      </c>
+      <c r="AE3" s="79">
+        <v>4017.8938145366546</v>
+      </c>
+      <c r="AF3" s="79">
+        <v>4003.5815606324636</v>
+      </c>
+      <c r="AG3" s="79">
+        <v>3988.9113124344767</v>
+      </c>
+      <c r="AH3" s="79">
+        <v>3943.6089504257593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="79">
+        <v>4740.3058669850725</v>
+      </c>
+      <c r="C4" s="79">
+        <v>4698.4718301828261</v>
+      </c>
+      <c r="D4" s="79">
+        <v>4656.6377933805788</v>
+      </c>
+      <c r="E4" s="79">
+        <v>4614.8037565783325</v>
+      </c>
+      <c r="F4" s="79">
+        <v>4572.9697197760852</v>
+      </c>
+      <c r="G4" s="79">
+        <v>4492.3388421270865</v>
+      </c>
+      <c r="H4" s="79">
+        <v>4450.5048053248402</v>
+      </c>
+      <c r="I4" s="79">
+        <v>4425.919733817439</v>
+      </c>
+      <c r="J4" s="79">
+        <v>4401.1503622317005</v>
+      </c>
+      <c r="K4" s="79">
+        <v>4375.6027304194013</v>
+      </c>
+      <c r="L4" s="79">
+        <v>4353.7695723430206</v>
+      </c>
+      <c r="M4" s="79">
+        <v>4323.0632929515905</v>
+      </c>
+      <c r="N4" s="79">
+        <v>4303.5989948717279</v>
+      </c>
+      <c r="O4" s="79">
+        <v>4285.2818354981382</v>
+      </c>
+      <c r="P4" s="79">
+        <v>4262.0324883591757</v>
+      </c>
+      <c r="Q4" s="79">
+        <v>4242.8368257164166</v>
+      </c>
+      <c r="R4" s="79">
+        <v>4225.3148592700782</v>
+      </c>
+      <c r="S4" s="79">
+        <v>4204.5718557405344</v>
+      </c>
+      <c r="T4" s="79">
+        <v>4184.3718456945344</v>
+      </c>
+      <c r="U4" s="79">
+        <v>4165.798924455009</v>
+      </c>
+      <c r="V4" s="79">
+        <v>4152.0220751579782</v>
+      </c>
+      <c r="W4" s="79">
+        <v>4136.0312119601085</v>
+      </c>
+      <c r="X4" s="79">
+        <v>4120.5639552154853</v>
+      </c>
+      <c r="Y4" s="79">
+        <v>4109.3400307856145</v>
+      </c>
+      <c r="Z4" s="79">
+        <v>4088.851743916076</v>
+      </c>
+      <c r="AA4" s="79">
+        <v>4079.7552383590519</v>
+      </c>
+      <c r="AB4" s="79">
+        <v>4060.153754291312</v>
+      </c>
+      <c r="AC4" s="79">
+        <v>4050.1467204692653</v>
+      </c>
+      <c r="AD4" s="79">
+        <v>4032.1404971157867</v>
+      </c>
+      <c r="AE4" s="79">
+        <v>4017.8938145366546</v>
+      </c>
+      <c r="AF4" s="79">
+        <v>4003.5815606324636</v>
+      </c>
+      <c r="AG4" s="79">
+        <v>3988.9113124344767</v>
+      </c>
+      <c r="AH4" s="79">
+        <v>3943.6089504257593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="C5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="D5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="E5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="F5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="G5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="H5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="I5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="J5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="K5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="L5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="M5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="N5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="O5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="P5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Q5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="R5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="S5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="T5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="U5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="V5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="W5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="X5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Y5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Z5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AA5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AB5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AC5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AD5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AE5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AF5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AG5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AH5" s="76">
+        <v>56.070672261119995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="C6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="D6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="E6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="F6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="G6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="H6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="I6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="J6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="K6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="L6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="M6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="N6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="O6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="P6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Q6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="R6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="S6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="T6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="U6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="V6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="W6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="X6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Y6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Z6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AA6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AB6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AC6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AD6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AE6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AF6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AG6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AH6" s="76">
+        <v>56.070672261119995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="C7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="D7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="E7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="F7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="G7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="H7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="I7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="J7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="K7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="L7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="M7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="N7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="O7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="P7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Q7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="R7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="S7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="T7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="U7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="V7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="W7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="X7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Y7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="Z7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AA7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AB7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AC7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AD7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AE7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AF7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AG7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+      <c r="AH7" s="76">
+        <v>56.070672261119995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="C8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="D8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="E8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="F8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="G8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="H8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="I8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="J8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="K8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="L8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="M8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="N8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="O8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="P8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Q8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="R8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="S8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="T8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="U8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="V8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="W8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="X8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Y8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Z8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AA8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AB8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AC8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AD8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AE8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AF8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AG8" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AH8" s="79">
+        <v>7.88067459072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
+      <c r="A9" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="C9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="D9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="E9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="F9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="G9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="H9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="I9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="J9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="K9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="L9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="M9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="N9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="O9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="P9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Q9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="R9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="S9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="T9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="U9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="V9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="W9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="X9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Y9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Z9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AA9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AB9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AC9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AD9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AE9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AF9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AG9" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AH9" s="79">
+        <v>7.88067459072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
+      <c r="A10" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="C10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="D10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="E10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="F10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="G10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="H10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="I10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="J10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="K10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="L10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="M10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="N10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="O10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="P10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Q10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="R10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="S10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="T10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="U10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="V10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="W10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="X10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Y10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="Z10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AA10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AB10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AC10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AD10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AE10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AF10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AG10" s="79">
+        <v>7.88067459072</v>
+      </c>
+      <c r="AH10" s="79">
+        <v>7.88067459072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>